<commit_message>
refactor reporting to utils toolbox
</commit_message>
<xml_diff>
--- a/data/output/performance_metrics.xlsx
+++ b/data/output/performance_metrics.xlsx
@@ -9,6 +9,7 @@
   <sheets>
     <sheet name="metrics" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="confusion_matrix" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="per_class_accuracy" sheetId="3" state="visible" r:id="rId3"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -36,7 +37,7 @@
       <color rgb="00000000"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
@@ -55,22 +56,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="003787C0"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="00ABD0E6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="00C6DBEF"/>
+        <fgColor rgb="006AAED6"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="006AAED6"/>
+        <fgColor rgb="00C6DBEF"/>
       </patternFill>
     </fill>
   </fills>
@@ -92,7 +88,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
@@ -103,16 +99,13 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -512,16 +505,16 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>0.82</v>
+        <v>0.78</v>
       </c>
       <c r="B2" t="n">
-        <v>0.8496666666666667</v>
+        <v>0.8090000000000001</v>
       </c>
       <c r="C2" t="n">
-        <v>0.82</v>
+        <v>0.78</v>
       </c>
       <c r="D2" t="n">
-        <v>0.8230822510822512</v>
+        <v>0.7777777777777779</v>
       </c>
     </row>
   </sheetData>
@@ -687,7 +680,7 @@
         <v>0</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D3" s="3" t="n">
         <v>0</v>
@@ -698,8 +691,8 @@
       <c r="F3" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G3" s="3" t="n">
-        <v>0</v>
+      <c r="G3" s="5" t="n">
+        <v>1</v>
       </c>
       <c r="H3" s="3" t="n">
         <v>0</v>
@@ -713,8 +706,8 @@
       <c r="K3" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="L3" s="3" t="n">
-        <v>0</v>
+      <c r="L3" s="6" t="n">
+        <v>1</v>
       </c>
       <c r="M3" s="3" t="n">
         <v>0</v>
@@ -722,8 +715,8 @@
       <c r="N3" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="O3" s="5" t="n">
-        <v>1</v>
+      <c r="O3" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="P3" s="3" t="n">
         <v>0</v>
@@ -797,7 +790,7 @@
         <v>0</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F5" s="3" t="n">
         <v>0</v>
@@ -820,8 +813,8 @@
       <c r="L5" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="M5" s="2" t="n">
-        <v>1</v>
+      <c r="M5" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="N5" s="3" t="n">
         <v>0</v>
@@ -1025,8 +1018,8 @@
       <c r="K9" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="L9" s="4" t="n">
-        <v>1</v>
+      <c r="L9" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="M9" s="3" t="n">
         <v>0</v>
@@ -1037,8 +1030,8 @@
       <c r="O9" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="P9" s="3" t="n">
-        <v>0</v>
+      <c r="P9" s="4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="10">
@@ -1105,8 +1098,8 @@
       <c r="C11" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="D11" s="6" t="n">
-        <v>1</v>
+      <c r="D11" s="3" t="n">
+        <v>0</v>
       </c>
       <c r="E11" s="3" t="n">
         <v>0</v>
@@ -1135,8 +1128,8 @@
       <c r="M11" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="N11" s="3" t="n">
-        <v>0</v>
+      <c r="N11" s="4" t="n">
+        <v>1</v>
       </c>
       <c r="O11" s="3" t="n">
         <v>0</v>
@@ -1169,7 +1162,7 @@
       <c r="G12" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="H12" s="4" t="n">
+      <c r="H12" s="6" t="n">
         <v>1</v>
       </c>
       <c r="I12" s="3" t="n">
@@ -1347,10 +1340,10 @@
         <v>0</v>
       </c>
       <c r="O15" s="2" t="n">
-        <v>2</v>
-      </c>
-      <c r="P15" s="3" t="n">
-        <v>0</v>
+        <v>1</v>
+      </c>
+      <c r="P15" s="4" t="n">
+        <v>1</v>
       </c>
     </row>
     <row r="16">
@@ -1359,8 +1352,8 @@
           <t>using_laptop</t>
         </is>
       </c>
-      <c r="B16" s="7" t="n">
-        <v>2</v>
+      <c r="B16" s="4" t="n">
+        <v>1</v>
       </c>
       <c r="C16" s="3" t="n">
         <v>0</v>
@@ -1374,8 +1367,8 @@
       <c r="F16" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="G16" s="3" t="n">
-        <v>0</v>
+      <c r="G16" s="5" t="n">
+        <v>1</v>
       </c>
       <c r="H16" s="3" t="n">
         <v>0</v>
@@ -1383,8 +1376,8 @@
       <c r="I16" s="3" t="n">
         <v>0</v>
       </c>
-      <c r="J16" s="3" t="n">
-        <v>0</v>
+      <c r="J16" s="4" t="n">
+        <v>1</v>
       </c>
       <c r="K16" s="3" t="n">
         <v>0</v>
@@ -1402,7 +1395,188 @@
         <v>0</v>
       </c>
       <c r="P16" s="2" t="n">
-        <v>4</v>
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:B16"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>class</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>accuracy</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>cycling</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>drinking</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>dancing</t>
+        </is>
+      </c>
+      <c r="B4" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>eating</t>
+        </is>
+      </c>
+      <c r="B5" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>fighting</t>
+        </is>
+      </c>
+      <c r="B6" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>sitting</t>
+        </is>
+      </c>
+      <c r="B7" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>laughing</t>
+        </is>
+      </c>
+      <c r="B8" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>running</t>
+        </is>
+      </c>
+      <c r="B9" t="n">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>calling</t>
+        </is>
+      </c>
+      <c r="B10" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>sleeping</t>
+        </is>
+      </c>
+      <c r="B11" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>listening_to_music</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>clapping</t>
+        </is>
+      </c>
+      <c r="B13" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>hugging</t>
+        </is>
+      </c>
+      <c r="B14" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>texting</t>
+        </is>
+      </c>
+      <c r="B15" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>using_laptop</t>
+        </is>
+      </c>
+      <c r="B16" t="n">
+        <v>0.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>